<commit_message>
Add RequireStall signal to Memories
</commit_message>
<xml_diff>
--- a/真值表.xlsx
+++ b/真值表.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76906D7E-168A-4F09-95EF-07442377EF6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FBA575-6207-4CD3-B33C-42D1BCCEB864}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3CF49F1C-E371-4F58-9CED-100EC43E1B66}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3CF49F1C-E371-4F58-9CED-100EC43E1B66}"/>
   </bookViews>
   <sheets>
     <sheet name="PipelineRegs" sheetId="9" r:id="rId1"/>
     <sheet name="Control" sheetId="4" r:id="rId2"/>
-    <sheet name="Branch" sheetId="2" r:id="rId3"/>
-    <sheet name="ALU" sheetId="1" r:id="rId4"/>
-    <sheet name="MulDiv" sheetId="5" r:id="rId5"/>
-    <sheet name="DataMemory" sheetId="3" r:id="rId6"/>
-    <sheet name="RegFile" sheetId="6" r:id="rId7"/>
-    <sheet name="HiLo" sheetId="8" r:id="rId8"/>
+    <sheet name="ControlException" sheetId="10" r:id="rId3"/>
+    <sheet name="Branch" sheetId="2" r:id="rId4"/>
+    <sheet name="ALU" sheetId="1" r:id="rId5"/>
+    <sheet name="MulDiv" sheetId="5" r:id="rId6"/>
+    <sheet name="DataMemory" sheetId="3" r:id="rId7"/>
+    <sheet name="RegFile" sheetId="6" r:id="rId8"/>
+    <sheet name="HiLo" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="182">
   <si>
     <t>触发整形溢出例外</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -721,6 +722,26 @@
   </si>
   <si>
     <t>takeEret</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exception</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无异常</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未知指令</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unknown</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -769,7 +790,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -794,6 +815,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -809,7 +848,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -936,16 +975,31 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1264,7 +1318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF38BED-6890-44F8-A207-BB1D25B80CDD}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1597,9 +1651,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BBE90BA-5E44-4EA5-9F54-AA356AE7D912}">
-  <dimension ref="A1:AA61"/>
+  <dimension ref="A1:AB62"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="7" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -1608,7 +1662,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5" style="20" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="6.5" style="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.5" style="20" bestFit="1" customWidth="1"/>
@@ -1624,112 +1678,115 @@
     <col min="18" max="18" width="10.125" style="19" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.25" style="24" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.625" style="19" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.375" style="19" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.875" style="24" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.375" style="23" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8" style="24" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11" style="22" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.125" style="22" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.875" style="19" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="9" style="19"/>
+    <col min="21" max="21" width="8.875" style="19" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.375" style="19" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.875" style="24" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.375" style="23" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8" style="24" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11" style="22" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.125" style="22" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.875" style="24" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="42" t="s">
+    <row r="1" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42" t="s">
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42" t="s">
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="42" t="s">
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="V1" s="42"/>
-      <c r="W1" s="42"/>
-      <c r="X1" s="42"/>
-      <c r="Y1" s="42"/>
-      <c r="Z1" s="42"/>
-      <c r="AA1" s="42"/>
-    </row>
-    <row r="2" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42" t="s">
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="42"/>
+    </row>
+    <row r="2" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42" t="s">
+      <c r="I2" s="44"/>
+      <c r="J2" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="K2" s="42"/>
+      <c r="K2" s="44"/>
       <c r="L2" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="M2" s="42" t="s">
+      <c r="M2" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
       <c r="P2" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="Q2" s="42" t="s">
+      <c r="Q2" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="R2" s="42"/>
-      <c r="S2" s="42"/>
-      <c r="T2" s="42"/>
-      <c r="U2" s="42" t="s">
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="V2" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="V2" s="42"/>
-      <c r="W2" s="42"/>
-      <c r="X2" s="44" t="s">
+      <c r="W2" s="44"/>
+      <c r="X2" s="44"/>
+      <c r="Y2" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="Y2" s="44"/>
-      <c r="Z2" s="44"/>
-      <c r="AA2" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
+      <c r="Z2" s="45"/>
+      <c r="AA2" s="45"/>
+      <c r="AB2" s="42"/>
+    </row>
+    <row r="3" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
       <c r="H3" s="14" t="s">
         <v>107</v>
       </c>
@@ -1770,28 +1827,31 @@
         <v>117</v>
       </c>
       <c r="U3" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="V3" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="W3" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="W3" s="18" t="s">
+      <c r="X3" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="X3" s="15" t="s">
+      <c r="Y3" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="Y3" s="17" t="s">
+      <c r="Z3" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="Z3" s="17" t="s">
+      <c r="AA3" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="AA3" s="14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AB3" s="42" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>156</v>
       </c>
@@ -1856,26 +1916,29 @@
         <v>1</v>
       </c>
       <c r="V4" s="17">
+        <v>1</v>
+      </c>
+      <c r="W4" s="17">
         <v>2</v>
       </c>
-      <c r="W4" s="17">
+      <c r="X4" s="17">
         <v>3</v>
       </c>
-      <c r="X4" s="17">
+      <c r="Y4" s="17">
         <v>2</v>
       </c>
-      <c r="Y4" s="17">
-        <v>1</v>
-      </c>
       <c r="Z4" s="17">
         <v>1</v>
       </c>
       <c r="AA4" s="17">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="AB4" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" s="48" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="20">
@@ -1936,29 +1999,29 @@
         <v>109</v>
       </c>
       <c r="U5" s="19">
-        <v>1</v>
-      </c>
-      <c r="V5" s="24">
-        <v>0</v>
-      </c>
-      <c r="W5" s="23">
-        <v>0</v>
-      </c>
-      <c r="X5" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V5" s="19">
+        <v>1</v>
+      </c>
+      <c r="W5" s="24">
+        <v>0</v>
+      </c>
+      <c r="X5" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="24">
+        <v>0</v>
       </c>
       <c r="Z5" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA5" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="AA5" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" s="48" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="20">
@@ -1970,11 +2033,11 @@
       <c r="D6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
       <c r="H6" s="19">
         <v>0</v>
       </c>
@@ -2015,29 +2078,29 @@
         <v>109</v>
       </c>
       <c r="U6" s="19">
-        <v>1</v>
-      </c>
-      <c r="V6" s="24">
-        <v>1</v>
-      </c>
-      <c r="W6" s="23">
-        <v>0</v>
-      </c>
-      <c r="X6" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V6" s="19">
+        <v>1</v>
+      </c>
+      <c r="W6" s="24">
+        <v>1</v>
+      </c>
+      <c r="X6" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="24">
+        <v>0</v>
       </c>
       <c r="Z6" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA6" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="AA6" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7" s="48" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="20">
@@ -2098,29 +2161,29 @@
         <v>109</v>
       </c>
       <c r="U7" s="19">
-        <v>1</v>
-      </c>
-      <c r="V7" s="24">
-        <v>0</v>
-      </c>
-      <c r="W7" s="23">
-        <v>0</v>
-      </c>
-      <c r="X7" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V7" s="19">
+        <v>1</v>
+      </c>
+      <c r="W7" s="24">
+        <v>0</v>
+      </c>
+      <c r="X7" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="24">
+        <v>0</v>
       </c>
       <c r="Z7" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA7" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="AA7" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8" s="48" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="20">
@@ -2132,11 +2195,11 @@
       <c r="D8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
       <c r="H8" s="19">
         <v>0</v>
       </c>
@@ -2177,29 +2240,29 @@
         <v>109</v>
       </c>
       <c r="U8" s="19">
-        <v>1</v>
-      </c>
-      <c r="V8" s="24">
-        <v>1</v>
-      </c>
-      <c r="W8" s="23">
-        <v>0</v>
-      </c>
-      <c r="X8" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V8" s="19">
+        <v>1</v>
+      </c>
+      <c r="W8" s="24">
+        <v>1</v>
+      </c>
+      <c r="X8" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="24">
+        <v>0</v>
       </c>
       <c r="Z8" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA8" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="AA8" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9" s="48" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="20">
@@ -2260,29 +2323,29 @@
         <v>109</v>
       </c>
       <c r="U9" s="19">
-        <v>1</v>
-      </c>
-      <c r="V9" s="24">
-        <v>0</v>
-      </c>
-      <c r="W9" s="23">
-        <v>0</v>
-      </c>
-      <c r="X9" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V9" s="19">
+        <v>1</v>
+      </c>
+      <c r="W9" s="24">
+        <v>0</v>
+      </c>
+      <c r="X9" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="24">
+        <v>0</v>
       </c>
       <c r="Z9" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA9" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="AA9" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A10" s="48" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="20">
@@ -2343,29 +2406,29 @@
         <v>109</v>
       </c>
       <c r="U10" s="19">
-        <v>1</v>
-      </c>
-      <c r="V10" s="24">
-        <v>0</v>
-      </c>
-      <c r="W10" s="23">
-        <v>0</v>
-      </c>
-      <c r="X10" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V10" s="19">
+        <v>1</v>
+      </c>
+      <c r="W10" s="24">
+        <v>0</v>
+      </c>
+      <c r="X10" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="24">
+        <v>0</v>
       </c>
       <c r="Z10" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA10" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
+      <c r="AA10" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A11" s="48" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="20">
@@ -2426,29 +2489,29 @@
         <v>109</v>
       </c>
       <c r="U11" s="19">
-        <v>1</v>
-      </c>
-      <c r="V11" s="24">
-        <v>0</v>
-      </c>
-      <c r="W11" s="23">
-        <v>0</v>
-      </c>
-      <c r="X11" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V11" s="19">
+        <v>1</v>
+      </c>
+      <c r="W11" s="24">
+        <v>0</v>
+      </c>
+      <c r="X11" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="24">
+        <v>0</v>
       </c>
       <c r="Z11" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA11" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
+      <c r="AA11" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A12" s="48" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="20">
@@ -2460,11 +2523,11 @@
       <c r="D12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
       <c r="H12" s="19">
         <v>0</v>
       </c>
@@ -2505,29 +2568,29 @@
         <v>109</v>
       </c>
       <c r="U12" s="19">
-        <v>1</v>
-      </c>
-      <c r="V12" s="24">
-        <v>1</v>
-      </c>
-      <c r="W12" s="23">
-        <v>0</v>
-      </c>
-      <c r="X12" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V12" s="19">
+        <v>1</v>
+      </c>
+      <c r="W12" s="24">
+        <v>1</v>
+      </c>
+      <c r="X12" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="24">
+        <v>0</v>
       </c>
       <c r="Z12" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA12" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
+      <c r="AA12" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A13" s="48" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="20">
@@ -2588,29 +2651,29 @@
         <v>109</v>
       </c>
       <c r="U13" s="19">
-        <v>1</v>
-      </c>
-      <c r="V13" s="24">
-        <v>0</v>
-      </c>
-      <c r="W13" s="23">
-        <v>0</v>
-      </c>
-      <c r="X13" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V13" s="19">
+        <v>1</v>
+      </c>
+      <c r="W13" s="24">
+        <v>0</v>
+      </c>
+      <c r="X13" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="24">
+        <v>0</v>
       </c>
       <c r="Z13" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA13" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+      <c r="AA13" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A14" s="48" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="20">
@@ -2622,11 +2685,11 @@
       <c r="D14" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
       <c r="H14" s="19">
         <v>0</v>
       </c>
@@ -2667,29 +2730,29 @@
         <v>109</v>
       </c>
       <c r="U14" s="19">
-        <v>1</v>
-      </c>
-      <c r="V14" s="24">
-        <v>1</v>
-      </c>
-      <c r="W14" s="23">
-        <v>0</v>
-      </c>
-      <c r="X14" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V14" s="19">
+        <v>1</v>
+      </c>
+      <c r="W14" s="24">
+        <v>1</v>
+      </c>
+      <c r="X14" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="24">
+        <v>0</v>
       </c>
       <c r="Z14" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA14" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+      <c r="AA14" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A15" s="48" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="20">
@@ -2752,27 +2815,27 @@
       <c r="U15" s="19">
         <v>0</v>
       </c>
-      <c r="V15" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W15" s="23" t="s">
+      <c r="V15" s="19">
+        <v>0</v>
+      </c>
+      <c r="W15" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X15" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X15" s="24">
+      <c r="Y15" s="24">
         <v>11</v>
       </c>
-      <c r="Y15" s="22">
-        <v>0</v>
-      </c>
       <c r="Z15" s="22">
         <v>0</v>
       </c>
-      <c r="AA15" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
+      <c r="AA15" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A16" s="48" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="20">
@@ -2835,27 +2898,27 @@
       <c r="U16" s="19">
         <v>0</v>
       </c>
-      <c r="V16" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W16" s="23" t="s">
+      <c r="V16" s="19">
+        <v>0</v>
+      </c>
+      <c r="W16" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X16" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X16" s="24">
+      <c r="Y16" s="24">
         <v>11</v>
       </c>
-      <c r="Y16" s="22">
-        <v>0</v>
-      </c>
       <c r="Z16" s="22">
         <v>0</v>
       </c>
-      <c r="AA16" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+      <c r="AA16" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A17" s="48" t="s">
         <v>40</v>
       </c>
       <c r="B17" s="20">
@@ -2918,27 +2981,27 @@
       <c r="U17" s="19">
         <v>0</v>
       </c>
-      <c r="V17" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W17" s="23" t="s">
+      <c r="V17" s="19">
+        <v>0</v>
+      </c>
+      <c r="W17" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X17" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X17" s="24">
+      <c r="Y17" s="24">
         <v>11</v>
       </c>
-      <c r="Y17" s="22">
-        <v>0</v>
-      </c>
       <c r="Z17" s="22">
         <v>0</v>
       </c>
-      <c r="AA17" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
+      <c r="AA17" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A18" s="48" t="s">
         <v>41</v>
       </c>
       <c r="B18" s="20">
@@ -3001,27 +3064,27 @@
       <c r="U18" s="19">
         <v>0</v>
       </c>
-      <c r="V18" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W18" s="23" t="s">
+      <c r="V18" s="19">
+        <v>0</v>
+      </c>
+      <c r="W18" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X18" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X18" s="24">
+      <c r="Y18" s="24">
         <v>11</v>
       </c>
-      <c r="Y18" s="22">
-        <v>0</v>
-      </c>
       <c r="Z18" s="22">
         <v>0</v>
       </c>
-      <c r="AA18" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
+      <c r="AA18" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A19" s="48" t="s">
         <v>42</v>
       </c>
       <c r="B19" s="20">
@@ -3082,29 +3145,29 @@
         <v>109</v>
       </c>
       <c r="U19" s="19">
-        <v>1</v>
-      </c>
-      <c r="V19" s="24">
-        <v>0</v>
-      </c>
-      <c r="W19" s="23">
-        <v>0</v>
-      </c>
-      <c r="X19" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V19" s="19">
+        <v>1</v>
+      </c>
+      <c r="W19" s="24">
+        <v>0</v>
+      </c>
+      <c r="X19" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="24">
+        <v>0</v>
       </c>
       <c r="Z19" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA19" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A20" s="19" t="s">
+      <c r="AA19" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A20" s="48" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="20">
@@ -3116,11 +3179,11 @@
       <c r="D20" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="43" t="s">
+      <c r="E20" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
       <c r="H20" s="19">
         <v>0</v>
       </c>
@@ -3161,29 +3224,29 @@
         <v>109</v>
       </c>
       <c r="U20" s="19">
-        <v>1</v>
-      </c>
-      <c r="V20" s="24">
-        <v>1</v>
-      </c>
-      <c r="W20" s="23">
-        <v>0</v>
-      </c>
-      <c r="X20" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V20" s="19">
+        <v>1</v>
+      </c>
+      <c r="W20" s="24">
+        <v>1</v>
+      </c>
+      <c r="X20" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="24">
+        <v>0</v>
       </c>
       <c r="Z20" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA20" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A21" s="19" t="s">
+      <c r="AA20" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A21" s="48" t="s">
         <v>44</v>
       </c>
       <c r="B21" s="20">
@@ -3195,11 +3258,11 @@
       <c r="D21" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="43" t="s">
+      <c r="E21" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
       <c r="H21" s="19">
         <v>0</v>
       </c>
@@ -3240,29 +3303,29 @@
         <v>109</v>
       </c>
       <c r="U21" s="19">
-        <v>1</v>
-      </c>
-      <c r="V21" s="24">
-        <v>1</v>
-      </c>
-      <c r="W21" s="23">
-        <v>0</v>
-      </c>
-      <c r="X21" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V21" s="19">
+        <v>1</v>
+      </c>
+      <c r="W21" s="24">
+        <v>1</v>
+      </c>
+      <c r="X21" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="24">
+        <v>0</v>
       </c>
       <c r="Z21" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA21" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A22" s="19" t="s">
+      <c r="AA21" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A22" s="48" t="s">
         <v>45</v>
       </c>
       <c r="B22" s="20">
@@ -3323,29 +3386,29 @@
         <v>109</v>
       </c>
       <c r="U22" s="19">
-        <v>1</v>
-      </c>
-      <c r="V22" s="24">
-        <v>0</v>
-      </c>
-      <c r="W22" s="23">
-        <v>0</v>
-      </c>
-      <c r="X22" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V22" s="19">
+        <v>1</v>
+      </c>
+      <c r="W22" s="24">
+        <v>0</v>
+      </c>
+      <c r="X22" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="24">
+        <v>0</v>
       </c>
       <c r="Z22" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA22" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A23" s="19" t="s">
+      <c r="AA22" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A23" s="48" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="20">
@@ -3406,29 +3469,32 @@
         <v>109</v>
       </c>
       <c r="U23" s="19">
-        <v>1</v>
-      </c>
-      <c r="V23" s="24">
-        <v>0</v>
-      </c>
-      <c r="W23" s="23">
-        <v>0</v>
-      </c>
-      <c r="X23" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V23" s="19">
+        <v>1</v>
+      </c>
+      <c r="W23" s="24">
+        <v>0</v>
+      </c>
+      <c r="X23" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="24">
+        <v>0</v>
       </c>
       <c r="Z23" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA23" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
+      <c r="AA23" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB23" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A24" s="48" t="s">
         <v>47</v>
       </c>
       <c r="B24" s="20">
@@ -3440,11 +3506,11 @@
       <c r="D24" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
       <c r="H24" s="19">
         <v>0</v>
       </c>
@@ -3485,29 +3551,32 @@
         <v>109</v>
       </c>
       <c r="U24" s="19">
-        <v>1</v>
-      </c>
-      <c r="V24" s="24">
-        <v>1</v>
-      </c>
-      <c r="W24" s="23">
-        <v>0</v>
-      </c>
-      <c r="X24" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y24" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V24" s="19">
+        <v>1</v>
+      </c>
+      <c r="W24" s="24">
+        <v>1</v>
+      </c>
+      <c r="X24" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="24">
+        <v>0</v>
       </c>
       <c r="Z24" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA24" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A25" s="19" t="s">
+      <c r="AA24" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB24" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A25" s="48" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="20">
@@ -3568,29 +3637,32 @@
         <v>109</v>
       </c>
       <c r="U25" s="19">
-        <v>1</v>
-      </c>
-      <c r="V25" s="24">
-        <v>0</v>
-      </c>
-      <c r="W25" s="23">
-        <v>0</v>
-      </c>
-      <c r="X25" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y25" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V25" s="19">
+        <v>1</v>
+      </c>
+      <c r="W25" s="24">
+        <v>0</v>
+      </c>
+      <c r="X25" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="24">
+        <v>0</v>
       </c>
       <c r="Z25" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA25" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A26" s="19" t="s">
+      <c r="AA25" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB25" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A26" s="48" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="20">
@@ -3602,11 +3674,11 @@
       <c r="D26" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="43" t="s">
+      <c r="E26" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
       <c r="H26" s="19">
         <v>0</v>
       </c>
@@ -3647,29 +3719,32 @@
         <v>109</v>
       </c>
       <c r="U26" s="19">
-        <v>1</v>
-      </c>
-      <c r="V26" s="24">
-        <v>1</v>
-      </c>
-      <c r="W26" s="23">
-        <v>0</v>
-      </c>
-      <c r="X26" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y26" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V26" s="19">
+        <v>1</v>
+      </c>
+      <c r="W26" s="24">
+        <v>1</v>
+      </c>
+      <c r="X26" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="24">
+        <v>0</v>
       </c>
       <c r="Z26" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA26" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A27" s="19" t="s">
+      <c r="AA26" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB26" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A27" s="48" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="20">
@@ -3730,29 +3805,32 @@
         <v>109</v>
       </c>
       <c r="U27" s="19">
-        <v>1</v>
-      </c>
-      <c r="V27" s="24">
-        <v>0</v>
-      </c>
-      <c r="W27" s="23">
-        <v>0</v>
-      </c>
-      <c r="X27" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y27" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V27" s="19">
+        <v>1</v>
+      </c>
+      <c r="W27" s="24">
+        <v>0</v>
+      </c>
+      <c r="X27" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="24">
+        <v>0</v>
       </c>
       <c r="Z27" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA27" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A28" s="19" t="s">
+      <c r="AA27" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB27" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A28" s="48" t="s">
         <v>52</v>
       </c>
       <c r="B28" s="20">
@@ -3813,29 +3891,32 @@
         <v>109</v>
       </c>
       <c r="U28" s="19">
-        <v>1</v>
-      </c>
-      <c r="V28" s="24">
-        <v>0</v>
-      </c>
-      <c r="W28" s="23">
-        <v>0</v>
-      </c>
-      <c r="X28" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y28" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V28" s="19">
+        <v>1</v>
+      </c>
+      <c r="W28" s="24">
+        <v>0</v>
+      </c>
+      <c r="X28" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="24">
+        <v>0</v>
       </c>
       <c r="Z28" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA28" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A29" s="19" t="s">
+      <c r="AA28" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB28" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A29" s="48" t="s">
         <v>53</v>
       </c>
       <c r="B29" s="20">
@@ -3896,29 +3977,32 @@
         <v>109</v>
       </c>
       <c r="U29" s="19">
-        <v>1</v>
-      </c>
-      <c r="V29" s="24">
-        <v>0</v>
-      </c>
-      <c r="W29" s="23">
-        <v>0</v>
-      </c>
-      <c r="X29" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y29" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V29" s="19">
+        <v>1</v>
+      </c>
+      <c r="W29" s="24">
+        <v>0</v>
+      </c>
+      <c r="X29" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="24">
+        <v>0</v>
       </c>
       <c r="Z29" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA29" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A30" s="19" t="s">
+      <c r="AA29" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB29" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A30" s="48" t="s">
         <v>54</v>
       </c>
       <c r="B30" s="20">
@@ -3979,29 +4063,32 @@
         <v>109</v>
       </c>
       <c r="U30" s="19">
-        <v>1</v>
-      </c>
-      <c r="V30" s="24">
-        <v>0</v>
-      </c>
-      <c r="W30" s="23">
-        <v>0</v>
-      </c>
-      <c r="X30" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y30" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V30" s="19">
+        <v>1</v>
+      </c>
+      <c r="W30" s="24">
+        <v>0</v>
+      </c>
+      <c r="X30" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="24">
+        <v>0</v>
       </c>
       <c r="Z30" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA30" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A31" s="19" t="s">
+      <c r="AA30" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB30" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A31" s="48" t="s">
         <v>55</v>
       </c>
       <c r="B31" s="20">
@@ -4062,29 +4149,32 @@
         <v>109</v>
       </c>
       <c r="U31" s="19">
-        <v>1</v>
-      </c>
-      <c r="V31" s="24">
-        <v>0</v>
-      </c>
-      <c r="W31" s="23">
-        <v>0</v>
-      </c>
-      <c r="X31" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y31" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V31" s="19">
+        <v>1</v>
+      </c>
+      <c r="W31" s="24">
+        <v>0</v>
+      </c>
+      <c r="X31" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="24">
+        <v>0</v>
       </c>
       <c r="Z31" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA31" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A32" s="19" t="s">
+      <c r="AA31" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB31" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A32" s="48" t="s">
         <v>56</v>
       </c>
       <c r="B32" s="20">
@@ -4145,29 +4235,32 @@
         <v>109</v>
       </c>
       <c r="U32" s="19">
-        <v>1</v>
-      </c>
-      <c r="V32" s="24">
-        <v>0</v>
-      </c>
-      <c r="W32" s="23">
-        <v>0</v>
-      </c>
-      <c r="X32" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y32" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V32" s="19">
+        <v>1</v>
+      </c>
+      <c r="W32" s="24">
+        <v>0</v>
+      </c>
+      <c r="X32" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="24">
+        <v>0</v>
       </c>
       <c r="Z32" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA32" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A33" s="19" t="s">
+      <c r="AA32" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB32" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A33" s="50" t="s">
         <v>5</v>
       </c>
       <c r="B33" s="20">
@@ -4179,11 +4272,11 @@
       <c r="D33" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E33" s="43" t="s">
+      <c r="E33" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
       <c r="H33" s="19">
         <v>1</v>
       </c>
@@ -4226,27 +4319,30 @@
       <c r="U33" s="19">
         <v>0</v>
       </c>
-      <c r="V33" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W33" s="23" t="s">
+      <c r="V33" s="19">
+        <v>0</v>
+      </c>
+      <c r="W33" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X33" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X33" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y33" s="22" t="s">
-        <v>109</v>
+      <c r="Y33" s="24">
+        <v>0</v>
       </c>
       <c r="Z33" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA33" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A34" s="19" t="s">
+      <c r="AA33" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB33" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A34" s="50" t="s">
         <v>6</v>
       </c>
       <c r="B34" s="20">
@@ -4258,11 +4354,11 @@
       <c r="D34" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E34" s="43" t="s">
+      <c r="E34" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
       <c r="H34" s="19">
         <v>1</v>
       </c>
@@ -4305,27 +4401,30 @@
       <c r="U34" s="19">
         <v>0</v>
       </c>
-      <c r="V34" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W34" s="23" t="s">
+      <c r="V34" s="19">
+        <v>0</v>
+      </c>
+      <c r="W34" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X34" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X34" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y34" s="22" t="s">
-        <v>109</v>
+      <c r="Y34" s="24">
+        <v>0</v>
       </c>
       <c r="Z34" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA34" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A35" s="19" t="s">
+      <c r="AA34" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB34" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A35" s="50" t="s">
         <v>9</v>
       </c>
       <c r="B35" s="20">
@@ -4337,11 +4436,11 @@
       <c r="D35" s="12">
         <v>1</v>
       </c>
-      <c r="E35" s="43" t="s">
+      <c r="E35" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
       <c r="H35" s="19">
         <v>1</v>
       </c>
@@ -4384,27 +4483,30 @@
       <c r="U35" s="19">
         <v>0</v>
       </c>
-      <c r="V35" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W35" s="23" t="s">
+      <c r="V35" s="19">
+        <v>0</v>
+      </c>
+      <c r="W35" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X35" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X35" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y35" s="22" t="s">
-        <v>109</v>
+      <c r="Y35" s="24">
+        <v>0</v>
       </c>
       <c r="Z35" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA35" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A36" s="19" t="s">
+      <c r="AA35" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB35" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A36" s="50" t="s">
         <v>10</v>
       </c>
       <c r="B36" s="20">
@@ -4416,11 +4518,11 @@
       <c r="D36" s="12">
         <v>0</v>
       </c>
-      <c r="E36" s="43" t="s">
+      <c r="E36" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
       <c r="H36" s="19">
         <v>1</v>
       </c>
@@ -4463,27 +4565,30 @@
       <c r="U36" s="19">
         <v>0</v>
       </c>
-      <c r="V36" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W36" s="23" t="s">
+      <c r="V36" s="19">
+        <v>0</v>
+      </c>
+      <c r="W36" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X36" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X36" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y36" s="22" t="s">
-        <v>109</v>
+      <c r="Y36" s="24">
+        <v>0</v>
       </c>
       <c r="Z36" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA36" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="s">
+      <c r="AA36" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB36" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A37" s="50" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="20">
@@ -4495,11 +4600,11 @@
       <c r="D37" s="12">
         <v>0</v>
       </c>
-      <c r="E37" s="43" t="s">
+      <c r="E37" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
       <c r="H37" s="19">
         <v>1</v>
       </c>
@@ -4542,27 +4647,30 @@
       <c r="U37" s="19">
         <v>0</v>
       </c>
-      <c r="V37" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W37" s="23" t="s">
+      <c r="V37" s="19">
+        <v>0</v>
+      </c>
+      <c r="W37" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X37" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X37" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y37" s="22" t="s">
-        <v>109</v>
+      <c r="Y37" s="24">
+        <v>0</v>
       </c>
       <c r="Z37" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA37" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A38" s="19" t="s">
+      <c r="AA37" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB37" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A38" s="50" t="s">
         <v>14</v>
       </c>
       <c r="B38" s="20">
@@ -4574,11 +4682,11 @@
       <c r="D38" s="12">
         <v>0</v>
       </c>
-      <c r="E38" s="43" t="s">
+      <c r="E38" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="46"/>
       <c r="H38" s="19">
         <v>1</v>
       </c>
@@ -4621,27 +4729,30 @@
       <c r="U38" s="19">
         <v>0</v>
       </c>
-      <c r="V38" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W38" s="23" t="s">
+      <c r="V38" s="19">
+        <v>0</v>
+      </c>
+      <c r="W38" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X38" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X38" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y38" s="22" t="s">
-        <v>109</v>
+      <c r="Y38" s="24">
+        <v>0</v>
       </c>
       <c r="Z38" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA38" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A39" s="19" t="s">
+      <c r="AA38" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB38" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A39" s="50" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="20">
@@ -4653,11 +4764,11 @@
       <c r="D39" s="12">
         <v>10001</v>
       </c>
-      <c r="E39" s="43" t="s">
+      <c r="E39" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
       <c r="H39" s="19">
         <v>1</v>
       </c>
@@ -4698,29 +4809,32 @@
         <v>109</v>
       </c>
       <c r="U39" s="19">
-        <v>1</v>
-      </c>
-      <c r="V39" s="24">
+        <v>0</v>
+      </c>
+      <c r="V39" s="19">
+        <v>1</v>
+      </c>
+      <c r="W39" s="24">
         <v>10</v>
       </c>
-      <c r="W39" s="23">
-        <v>1</v>
-      </c>
-      <c r="X39" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y39" s="22" t="s">
-        <v>109</v>
+      <c r="X39" s="23">
+        <v>1</v>
+      </c>
+      <c r="Y39" s="24">
+        <v>0</v>
       </c>
       <c r="Z39" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA39" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A40" s="19" t="s">
+      <c r="AA39" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB39" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A40" s="50" t="s">
         <v>17</v>
       </c>
       <c r="B40" s="20">
@@ -4732,11 +4846,11 @@
       <c r="D40" s="12">
         <v>10000</v>
       </c>
-      <c r="E40" s="43" t="s">
+      <c r="E40" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
       <c r="H40" s="19">
         <v>1</v>
       </c>
@@ -4777,41 +4891,44 @@
         <v>109</v>
       </c>
       <c r="U40" s="19">
-        <v>1</v>
-      </c>
-      <c r="V40" s="24">
+        <v>0</v>
+      </c>
+      <c r="V40" s="19">
+        <v>1</v>
+      </c>
+      <c r="W40" s="24">
         <v>10</v>
       </c>
-      <c r="W40" s="23">
-        <v>1</v>
-      </c>
-      <c r="X40" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y40" s="22" t="s">
-        <v>109</v>
+      <c r="X40" s="23">
+        <v>1</v>
+      </c>
+      <c r="Y40" s="24">
+        <v>0</v>
       </c>
       <c r="Z40" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA40" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A41" s="19" t="s">
+      <c r="AA40" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB40" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A41" s="50" t="s">
         <v>57</v>
       </c>
       <c r="B41" s="20">
         <v>10</v>
       </c>
-      <c r="C41" s="43" t="s">
+      <c r="C41" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
       <c r="H41" s="19">
         <v>0</v>
       </c>
@@ -4854,39 +4971,42 @@
       <c r="U41" s="19">
         <v>0</v>
       </c>
-      <c r="V41" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W41" s="23" t="s">
+      <c r="V41" s="19">
+        <v>0</v>
+      </c>
+      <c r="W41" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X41" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X41" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y41" s="22" t="s">
-        <v>109</v>
+      <c r="Y41" s="24">
+        <v>0</v>
       </c>
       <c r="Z41" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA41" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A42" s="19" t="s">
+      <c r="AA41" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB41" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A42" s="50" t="s">
         <v>58</v>
       </c>
       <c r="B42" s="20">
         <v>11</v>
       </c>
-      <c r="C42" s="43" t="s">
+      <c r="C42" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="43"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
       <c r="H42" s="19">
         <v>0</v>
       </c>
@@ -4927,29 +5047,32 @@
         <v>109</v>
       </c>
       <c r="U42" s="19">
-        <v>1</v>
-      </c>
-      <c r="V42" s="24">
+        <v>0</v>
+      </c>
+      <c r="V42" s="19">
+        <v>1</v>
+      </c>
+      <c r="W42" s="24">
         <v>10</v>
       </c>
-      <c r="W42" s="23">
-        <v>1</v>
-      </c>
-      <c r="X42" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y42" s="22" t="s">
-        <v>109</v>
+      <c r="X42" s="23">
+        <v>1</v>
+      </c>
+      <c r="Y42" s="24">
+        <v>0</v>
       </c>
       <c r="Z42" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA42" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A43" s="19" t="s">
+      <c r="AA42" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB42" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A43" s="50" t="s">
         <v>59</v>
       </c>
       <c r="B43" s="20">
@@ -5012,27 +5135,30 @@
       <c r="U43" s="19">
         <v>0</v>
       </c>
-      <c r="V43" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W43" s="23" t="s">
+      <c r="V43" s="19">
+        <v>0</v>
+      </c>
+      <c r="W43" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X43" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X43" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y43" s="22" t="s">
-        <v>109</v>
+      <c r="Y43" s="24">
+        <v>0</v>
       </c>
       <c r="Z43" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA43" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A44" s="19" t="s">
+      <c r="AA43" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB43" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A44" s="50" t="s">
         <v>60</v>
       </c>
       <c r="B44" s="20">
@@ -5093,29 +5219,32 @@
         <v>109</v>
       </c>
       <c r="U44" s="19">
-        <v>1</v>
-      </c>
-      <c r="V44" s="24">
-        <v>0</v>
-      </c>
-      <c r="W44" s="23">
-        <v>1</v>
-      </c>
-      <c r="X44" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y44" s="22" t="s">
-        <v>109</v>
+        <v>0</v>
+      </c>
+      <c r="V44" s="19">
+        <v>1</v>
+      </c>
+      <c r="W44" s="24">
+        <v>0</v>
+      </c>
+      <c r="X44" s="23">
+        <v>1</v>
+      </c>
+      <c r="Y44" s="24">
+        <v>0</v>
       </c>
       <c r="Z44" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA44" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A45" s="19" t="s">
+      <c r="AA44" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB44" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A45" s="49" t="s">
         <v>61</v>
       </c>
       <c r="B45" s="20">
@@ -5176,29 +5305,32 @@
         <v>109</v>
       </c>
       <c r="U45" s="19">
-        <v>1</v>
-      </c>
-      <c r="V45" s="24">
-        <v>0</v>
-      </c>
-      <c r="W45" s="23">
+        <v>0</v>
+      </c>
+      <c r="V45" s="19">
+        <v>1</v>
+      </c>
+      <c r="W45" s="24">
+        <v>0</v>
+      </c>
+      <c r="X45" s="23">
         <v>10</v>
       </c>
-      <c r="X45" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y45" s="22" t="s">
-        <v>109</v>
+      <c r="Y45" s="24">
+        <v>0</v>
       </c>
       <c r="Z45" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA45" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A46" s="19" t="s">
+      <c r="AA45" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB45" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A46" s="49" t="s">
         <v>62</v>
       </c>
       <c r="B46" s="20">
@@ -5259,29 +5391,32 @@
         <v>109</v>
       </c>
       <c r="U46" s="19">
-        <v>1</v>
-      </c>
-      <c r="V46" s="24">
-        <v>0</v>
-      </c>
-      <c r="W46" s="23">
+        <v>0</v>
+      </c>
+      <c r="V46" s="19">
+        <v>1</v>
+      </c>
+      <c r="W46" s="24">
+        <v>0</v>
+      </c>
+      <c r="X46" s="23">
         <v>11</v>
       </c>
-      <c r="X46" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y46" s="22" t="s">
-        <v>109</v>
+      <c r="Y46" s="24">
+        <v>0</v>
       </c>
       <c r="Z46" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA46" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A47" s="19" t="s">
+      <c r="AA46" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB46" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A47" s="32" t="s">
         <v>63</v>
       </c>
       <c r="B47" s="20">
@@ -5344,27 +5479,30 @@
       <c r="U47" s="19">
         <v>0</v>
       </c>
-      <c r="V47" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W47" s="23" t="s">
+      <c r="V47" s="19">
+        <v>0</v>
+      </c>
+      <c r="W47" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X47" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X47" s="24">
+      <c r="Y47" s="24">
         <v>10</v>
       </c>
-      <c r="Y47" s="22">
-        <v>1</v>
-      </c>
-      <c r="Z47" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA47" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A48" s="19" t="s">
+      <c r="Z47" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA47" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB47" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A48" s="32" t="s">
         <v>64</v>
       </c>
       <c r="B48" s="20">
@@ -5427,38 +5565,41 @@
       <c r="U48" s="19">
         <v>0</v>
       </c>
-      <c r="V48" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W48" s="23" t="s">
+      <c r="V48" s="19">
+        <v>0</v>
+      </c>
+      <c r="W48" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X48" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X48" s="24">
-        <v>1</v>
-      </c>
-      <c r="Y48" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="Z48" s="22">
-        <v>1</v>
-      </c>
-      <c r="AA48" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Y48" s="24">
+        <v>1</v>
+      </c>
+      <c r="Z48" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA48" s="22">
+        <v>1</v>
+      </c>
+      <c r="AB48" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B49" s="20">
         <v>0</v>
       </c>
-      <c r="C49" s="43" t="s">
+      <c r="C49" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="D49" s="43"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="43"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="46"/>
       <c r="G49" s="20">
         <v>1101</v>
       </c>
@@ -5504,38 +5645,41 @@
       <c r="U49" s="19">
         <v>0</v>
       </c>
-      <c r="V49" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W49" s="23" t="s">
+      <c r="V49" s="19">
+        <v>0</v>
+      </c>
+      <c r="W49" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X49" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X49" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y49" s="22" t="s">
-        <v>109</v>
+      <c r="Y49" s="24">
+        <v>0</v>
       </c>
       <c r="Z49" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA49" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA49" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB49" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="s">
         <v>67</v>
       </c>
       <c r="B50" s="20">
         <v>0</v>
       </c>
-      <c r="C50" s="43" t="s">
+      <c r="C50" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
       <c r="G50" s="20">
         <v>1100</v>
       </c>
@@ -5581,26 +5725,29 @@
       <c r="U50" s="19">
         <v>0</v>
       </c>
-      <c r="V50" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W50" s="23" t="s">
+      <c r="V50" s="19">
+        <v>0</v>
+      </c>
+      <c r="W50" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X50" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X50" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y50" s="22" t="s">
-        <v>109</v>
+      <c r="Y50" s="24">
+        <v>0</v>
       </c>
       <c r="Z50" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA50" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA50" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB50" s="24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
         <v>68</v>
       </c>
@@ -5613,11 +5760,11 @@
       <c r="D51" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E51" s="43" t="s">
+      <c r="E51" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F51" s="43"/>
-      <c r="G51" s="43"/>
+      <c r="F51" s="46"/>
+      <c r="G51" s="46"/>
       <c r="H51" s="19">
         <v>0</v>
       </c>
@@ -5658,28 +5805,31 @@
         <v>1</v>
       </c>
       <c r="U51" s="19">
-        <v>1</v>
-      </c>
-      <c r="V51" s="24">
-        <v>1</v>
-      </c>
-      <c r="W51" s="23">
+        <v>0</v>
+      </c>
+      <c r="V51" s="19">
+        <v>1</v>
+      </c>
+      <c r="W51" s="24">
+        <v>1</v>
+      </c>
+      <c r="X51" s="23">
         <v>100</v>
       </c>
-      <c r="X51" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y51" s="22" t="s">
-        <v>109</v>
+      <c r="Y51" s="24">
+        <v>0</v>
       </c>
       <c r="Z51" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA51" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA51" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB51" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
         <v>69</v>
       </c>
@@ -5692,11 +5842,11 @@
       <c r="D52" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E52" s="43" t="s">
+      <c r="E52" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F52" s="43"/>
-      <c r="G52" s="43"/>
+      <c r="F52" s="46"/>
+      <c r="G52" s="46"/>
       <c r="H52" s="19">
         <v>0</v>
       </c>
@@ -5737,28 +5887,31 @@
         <v>0</v>
       </c>
       <c r="U52" s="19">
-        <v>1</v>
-      </c>
-      <c r="V52" s="24">
-        <v>1</v>
-      </c>
-      <c r="W52" s="23">
+        <v>0</v>
+      </c>
+      <c r="V52" s="19">
+        <v>1</v>
+      </c>
+      <c r="W52" s="24">
+        <v>1</v>
+      </c>
+      <c r="X52" s="23">
         <v>100</v>
       </c>
-      <c r="X52" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y52" s="22" t="s">
-        <v>109</v>
+      <c r="Y52" s="24">
+        <v>0</v>
       </c>
       <c r="Z52" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA52" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA52" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB52" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A53" s="19" t="s">
         <v>70</v>
       </c>
@@ -5771,11 +5924,11 @@
       <c r="D53" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E53" s="43" t="s">
+      <c r="E53" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F53" s="43"/>
-      <c r="G53" s="43"/>
+      <c r="F53" s="46"/>
+      <c r="G53" s="46"/>
       <c r="H53" s="19">
         <v>0</v>
       </c>
@@ -5816,28 +5969,31 @@
         <v>1</v>
       </c>
       <c r="U53" s="19">
-        <v>1</v>
-      </c>
-      <c r="V53" s="24">
-        <v>1</v>
-      </c>
-      <c r="W53" s="23">
+        <v>0</v>
+      </c>
+      <c r="V53" s="19">
+        <v>1</v>
+      </c>
+      <c r="W53" s="24">
+        <v>1</v>
+      </c>
+      <c r="X53" s="23">
         <v>100</v>
       </c>
-      <c r="X53" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y53" s="22" t="s">
-        <v>109</v>
+      <c r="Y53" s="24">
+        <v>0</v>
       </c>
       <c r="Z53" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA53" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA53" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB53" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="s">
         <v>71</v>
       </c>
@@ -5850,11 +6006,11 @@
       <c r="D54" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E54" s="43" t="s">
+      <c r="E54" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F54" s="43"/>
-      <c r="G54" s="43"/>
+      <c r="F54" s="46"/>
+      <c r="G54" s="46"/>
       <c r="H54" s="19">
         <v>0</v>
       </c>
@@ -5895,28 +6051,31 @@
         <v>0</v>
       </c>
       <c r="U54" s="19">
-        <v>1</v>
-      </c>
-      <c r="V54" s="24">
-        <v>1</v>
-      </c>
-      <c r="W54" s="23">
+        <v>0</v>
+      </c>
+      <c r="V54" s="19">
+        <v>1</v>
+      </c>
+      <c r="W54" s="24">
+        <v>1</v>
+      </c>
+      <c r="X54" s="23">
         <v>100</v>
       </c>
-      <c r="X54" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y54" s="22" t="s">
-        <v>109</v>
+      <c r="Y54" s="24">
+        <v>0</v>
       </c>
       <c r="Z54" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA54" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA54" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB54" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="s">
         <v>72</v>
       </c>
@@ -5929,11 +6088,11 @@
       <c r="D55" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E55" s="43" t="s">
+      <c r="E55" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F55" s="43"/>
-      <c r="G55" s="43"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="46"/>
       <c r="H55" s="19">
         <v>0</v>
       </c>
@@ -5974,28 +6133,31 @@
         <v>109</v>
       </c>
       <c r="U55" s="19">
-        <v>1</v>
-      </c>
-      <c r="V55" s="24">
-        <v>1</v>
-      </c>
-      <c r="W55" s="23">
+        <v>0</v>
+      </c>
+      <c r="V55" s="19">
+        <v>1</v>
+      </c>
+      <c r="W55" s="24">
+        <v>1</v>
+      </c>
+      <c r="X55" s="23">
         <v>100</v>
       </c>
-      <c r="X55" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y55" s="22" t="s">
-        <v>109</v>
+      <c r="Y55" s="24">
+        <v>0</v>
       </c>
       <c r="Z55" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA55" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA55" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB55" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
         <v>73</v>
       </c>
@@ -6008,11 +6170,11 @@
       <c r="D56" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E56" s="43" t="s">
+      <c r="E56" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
+      <c r="F56" s="46"/>
+      <c r="G56" s="46"/>
       <c r="H56" s="19">
         <v>0</v>
       </c>
@@ -6055,26 +6217,29 @@
       <c r="U56" s="19">
         <v>0</v>
       </c>
-      <c r="V56" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W56" s="23" t="s">
+      <c r="V56" s="19">
+        <v>0</v>
+      </c>
+      <c r="W56" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X56" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X56" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y56" s="22" t="s">
-        <v>109</v>
+      <c r="Y56" s="24">
+        <v>0</v>
       </c>
       <c r="Z56" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA56" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA56" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB56" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="s">
         <v>74</v>
       </c>
@@ -6087,11 +6252,11 @@
       <c r="D57" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E57" s="43" t="s">
+      <c r="E57" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
       <c r="H57" s="19">
         <v>0</v>
       </c>
@@ -6134,26 +6299,29 @@
       <c r="U57" s="19">
         <v>0</v>
       </c>
-      <c r="V57" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W57" s="23" t="s">
+      <c r="V57" s="19">
+        <v>0</v>
+      </c>
+      <c r="W57" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X57" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X57" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y57" s="22" t="s">
-        <v>109</v>
+      <c r="Y57" s="24">
+        <v>0</v>
       </c>
       <c r="Z57" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA57" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA57" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB57" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
         <v>75</v>
       </c>
@@ -6166,11 +6334,11 @@
       <c r="D58" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E58" s="43" t="s">
+      <c r="E58" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F58" s="43"/>
-      <c r="G58" s="43"/>
+      <c r="F58" s="46"/>
+      <c r="G58" s="46"/>
       <c r="H58" s="19">
         <v>0</v>
       </c>
@@ -6213,26 +6381,29 @@
       <c r="U58" s="19">
         <v>0</v>
       </c>
-      <c r="V58" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W58" s="23" t="s">
+      <c r="V58" s="19">
+        <v>0</v>
+      </c>
+      <c r="W58" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X58" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X58" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y58" s="22" t="s">
-        <v>109</v>
+      <c r="Y58" s="24">
+        <v>0</v>
       </c>
       <c r="Z58" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA58" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA58" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB58" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="s">
         <v>76</v>
       </c>
@@ -6294,29 +6465,32 @@
         <v>109</v>
       </c>
       <c r="U59" s="19">
-        <v>0</v>
-      </c>
-      <c r="V59" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W59" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="V59" s="19">
+        <v>0</v>
+      </c>
+      <c r="W59" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X59" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X59" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y59" s="22" t="s">
-        <v>109</v>
+      <c r="Y59" s="24">
+        <v>0</v>
       </c>
       <c r="Z59" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA59" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A60" s="19" t="s">
+      <c r="AA59" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB59" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A60" s="49" t="s">
         <v>78</v>
       </c>
       <c r="B60" s="20">
@@ -6377,29 +6551,32 @@
         <v>109</v>
       </c>
       <c r="U60" s="19">
-        <v>1</v>
-      </c>
-      <c r="V60" s="24">
-        <v>1</v>
-      </c>
-      <c r="W60" s="23">
+        <v>0</v>
+      </c>
+      <c r="V60" s="19">
+        <v>1</v>
+      </c>
+      <c r="W60" s="24">
+        <v>1</v>
+      </c>
+      <c r="X60" s="23">
         <v>101</v>
       </c>
-      <c r="X60" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y60" s="22" t="s">
-        <v>109</v>
+      <c r="Y60" s="24">
+        <v>0</v>
       </c>
       <c r="Z60" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA60" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A61" s="19" t="s">
+      <c r="AA60" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB60" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A61" s="32" t="s">
         <v>79</v>
       </c>
       <c r="B61" s="20">
@@ -6462,54 +6639,98 @@
       <c r="U61" s="19">
         <v>0</v>
       </c>
-      <c r="V61" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="W61" s="23" t="s">
+      <c r="V61" s="19">
+        <v>0</v>
+      </c>
+      <c r="W61" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X61" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="X61" s="24">
-        <v>0</v>
-      </c>
-      <c r="Y61" s="22" t="s">
-        <v>109</v>
+      <c r="Y61" s="24">
+        <v>0</v>
       </c>
       <c r="Z61" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AA61" s="19">
-        <v>0</v>
+      <c r="AA61" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB61" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A62" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="H62" s="19">
+        <v>0</v>
+      </c>
+      <c r="I62" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="J62" s="19">
+        <v>0</v>
+      </c>
+      <c r="K62" s="19">
+        <v>0</v>
+      </c>
+      <c r="L62" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="M62" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="N62" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="O62" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="P62" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q62" s="19">
+        <v>0</v>
+      </c>
+      <c r="R62" s="19">
+        <v>0</v>
+      </c>
+      <c r="S62" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="T62" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="U62" s="19">
+        <v>0</v>
+      </c>
+      <c r="V62" s="19">
+        <v>0</v>
+      </c>
+      <c r="W62" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="X62" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y62" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z62" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA62" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB62" s="24">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="U1:AA1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="M1:P1"/>
-    <mergeCell ref="Q1:T1"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:G3"/>
     <mergeCell ref="E35:G35"/>
@@ -6523,14 +6744,147 @@
     <mergeCell ref="E26:G26"/>
     <mergeCell ref="E33:G33"/>
     <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="V1:AA1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="V1:V61 V63:V1048576">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M1:M61 M63:M1048576">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V62">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M62">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1455F1E-27B3-46CA-8480-0FA685041C4F}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="9"/>
+    <col min="2" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="9">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D6B0BF-8614-43A7-9F15-E4FE95337B3D}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -6551,10 +6905,10 @@
       <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="45"/>
+      <c r="B1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="47"/>
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
@@ -6640,7 +6994,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDACB7E2-4D21-4756-8FC0-21D4AFA9E8B8}">
   <dimension ref="A1:K15"/>
   <sheetViews>
@@ -6668,11 +7022,11 @@
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
+      <c r="B1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
@@ -6925,7 +7279,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57FB907F-79B3-4E46-B52E-E717521277CF}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -6986,7 +7340,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD702E6A-ACE3-4E0D-8A99-CB82ACE23858}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -7037,7 +7391,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{947260C0-B57D-402D-A7FB-E56302B48C32}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -7146,7 +7500,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780E22FF-6159-4733-93EB-5184B9746FE9}">
   <dimension ref="A1:E3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Finish MIPS without hazard/exception, not tested
</commit_message>
<xml_diff>
--- a/真值表.xlsx
+++ b/真值表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8F4082-B19D-481F-B540-A7C53969A4A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74E0067-06DA-43EA-9399-A6C3285E0A01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3CF49F1C-E371-4F58-9CED-100EC43E1B66}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{3CF49F1C-E371-4F58-9CED-100EC43E1B66}"/>
   </bookViews>
   <sheets>
     <sheet name="PipelineRegs" sheetId="9" r:id="rId1"/>
@@ -20,8 +20,8 @@
     <sheet name="ALU" sheetId="1" r:id="rId5"/>
     <sheet name="MulDiv" sheetId="5" r:id="rId6"/>
     <sheet name="DataMemory" sheetId="3" r:id="rId7"/>
-    <sheet name="RegFile" sheetId="6" r:id="rId8"/>
-    <sheet name="HiLo" sheetId="8" r:id="rId9"/>
+    <sheet name="HiLo" sheetId="8" r:id="rId8"/>
+    <sheet name="RegFile" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="193">
   <si>
     <t>触发整形溢出例外</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -569,14 +569,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Hi</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DmDout</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -721,10 +713,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>takeEret</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Exception</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -742,6 +730,62 @@
   </si>
   <si>
     <t>unknown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CP0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cp0Write</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cp0Write</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>regDout1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>regDout2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aluDout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mdDoutHi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mdDoutLo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HlDoutHi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HlDoutLo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hlDoutHi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hlDoutLo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dmDout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cp0Dout</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -848,7 +892,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -967,12 +1011,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1319,9 +1357,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF38BED-6890-44F8-A207-BB1D25B80CDD}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1341,51 +1381,51 @@
   <sheetData>
     <row r="1" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="E1" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="H1" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="J1" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="E1" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="J1" s="25" t="s">
-        <v>159</v>
-      </c>
       <c r="K1" s="25" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B2" s="1">
         <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E2" s="1">
         <v>32</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H2" s="1">
         <v>32</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K2" s="1">
         <v>32</v>
@@ -1393,255 +1433,363 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B3" s="1">
         <v>32</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E3" s="1">
         <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H3" s="1">
         <v>32</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K3" s="1">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E4" s="1">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H4" s="1">
+        <v>32</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="K4" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D5" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E5" s="1">
+        <v>32</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H5" s="1">
+        <v>32</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="K5" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D6" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="1">
+        <v>32</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H6" s="1">
+        <v>32</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="K6" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D7" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" s="32">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H7" s="1">
+        <v>32</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="K7" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D8" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="E8" s="32">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H8" s="1">
+        <v>32</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="K8" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D9" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="E4" s="32">
-        <v>4</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>166</v>
-      </c>
-      <c r="H4" s="30">
-        <v>1</v>
-      </c>
-      <c r="J4" s="38" t="s">
-        <v>170</v>
-      </c>
-      <c r="K4" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D5" s="34" t="s">
+      <c r="E9" s="32">
+        <v>1</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="H9" s="30">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="K9" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D10" s="35" t="s">
         <v>163</v>
       </c>
-      <c r="E5" s="32">
-        <v>1</v>
-      </c>
-      <c r="G5" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="H5" s="30">
-        <v>1</v>
-      </c>
-      <c r="J5" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="K5" s="31">
+      <c r="E10" s="32">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D6" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="E6" s="32">
-        <v>1</v>
-      </c>
-      <c r="G6" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="H6" s="30">
-        <v>2</v>
-      </c>
-      <c r="J6" s="40" t="s">
-        <v>172</v>
-      </c>
-      <c r="K6" s="31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D7" s="35" t="s">
+      <c r="G10" s="36" t="s">
         <v>165</v>
       </c>
-      <c r="E7" s="32">
-        <v>2</v>
-      </c>
-      <c r="G7" s="36" t="s">
-        <v>169</v>
-      </c>
-      <c r="H7" s="30">
-        <v>1</v>
-      </c>
-      <c r="J7" s="39" t="s">
-        <v>173</v>
-      </c>
-      <c r="K7" s="31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D8" s="36" t="s">
-        <v>166</v>
-      </c>
-      <c r="E8" s="30">
-        <v>1</v>
-      </c>
-      <c r="G8" s="38" t="s">
-        <v>170</v>
-      </c>
-      <c r="H8" s="31">
-        <v>1</v>
-      </c>
-      <c r="J8" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="K8" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D9" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="E9" s="30">
-        <v>1</v>
-      </c>
-      <c r="G9" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="H9" s="31">
-        <v>2</v>
-      </c>
-      <c r="J9" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="K9" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D10" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="E10" s="30">
-        <v>2</v>
-      </c>
-      <c r="G10" s="40" t="s">
-        <v>172</v>
-      </c>
-      <c r="H10" s="31">
-        <v>3</v>
-      </c>
-      <c r="J10" s="38" t="s">
-        <v>176</v>
-      </c>
-      <c r="K10" s="31">
-        <v>1</v>
+      <c r="H10" s="30">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="K10" s="1">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D11" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="E11" s="30">
+        <v>1</v>
+      </c>
+      <c r="G11" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="H11" s="30">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K11" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D12" s="36" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" s="30">
+        <v>1</v>
+      </c>
+      <c r="G12" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="H12" s="30">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="K12" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D13" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="E13" s="30">
+        <v>2</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="H13" s="31">
+        <v>1</v>
+      </c>
+      <c r="J13" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="K13" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D14" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="E14" s="30">
+        <v>1</v>
+      </c>
+      <c r="G14" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="E11" s="30">
-        <v>1</v>
-      </c>
-      <c r="G11" s="39" t="s">
+      <c r="H14" s="31">
+        <v>2</v>
+      </c>
+      <c r="J14" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="K14" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D15" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="E15" s="31">
+        <v>1</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="H15" s="31">
+        <v>3</v>
+      </c>
+      <c r="J15" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="K15" s="31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D16" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="E16" s="31">
+        <v>2</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="H16" s="31">
+        <v>1</v>
+      </c>
+      <c r="J16" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="K16" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D17" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="E17" s="31">
+        <v>3</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="H17" s="31">
+        <v>2</v>
+      </c>
+      <c r="J17" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="K17" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D18" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="E18" s="31">
+        <v>1</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="H18" s="31">
+        <v>1</v>
+      </c>
+      <c r="J18" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="K18" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D19" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="E19" s="31">
+        <v>2</v>
+      </c>
+      <c r="G19" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="H11" s="31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D12" s="38" t="s">
-        <v>170</v>
-      </c>
-      <c r="E12" s="31">
-        <v>1</v>
-      </c>
-      <c r="G12" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="H12" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D13" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="E13" s="31">
-        <v>2</v>
-      </c>
-      <c r="G13" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="H13" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D14" s="40" t="s">
+      <c r="H19" s="31">
+        <v>1</v>
+      </c>
+      <c r="J19" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="K19" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D20" s="31" t="s">
         <v>172</v>
       </c>
-      <c r="E14" s="31">
-        <v>3</v>
-      </c>
-      <c r="G14" s="38" t="s">
-        <v>176</v>
-      </c>
-      <c r="H14" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D15" s="39" t="s">
+      <c r="E20" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D21" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="E15" s="31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D16" s="41" t="s">
-        <v>174</v>
-      </c>
-      <c r="E16" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D17" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="E17" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D18" s="38" t="s">
-        <v>176</v>
-      </c>
-      <c r="E18" s="31">
+      <c r="E21" s="31">
         <v>1</v>
       </c>
     </row>
@@ -1654,13 +1802,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BBE90BA-5E44-4EA5-9F54-AA356AE7D912}">
-  <dimension ref="A1:AB62"/>
+  <dimension ref="A1:AC62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="7" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1685,125 +1833,130 @@
     <col min="22" max="22" width="9.375" style="19" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12.875" style="24" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10.375" style="23" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8" style="24" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11" style="22" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.125" style="22" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.875" style="24" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="9" style="19"/>
+    <col min="25" max="25" width="10.375" style="22" customWidth="1"/>
+    <col min="26" max="26" width="8" style="24" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11" style="22" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.125" style="22" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.875" style="24" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="45" t="s">
+    <row r="1" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45" t="s">
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45" t="s">
-        <v>143</v>
-      </c>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45" t="s">
-        <v>145</v>
-      </c>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45" t="s">
-        <v>146</v>
-      </c>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="45"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43"/>
+      <c r="AA1" s="43"/>
       <c r="AB1" s="43"/>
-    </row>
-    <row r="2" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45" t="s">
+      <c r="AC1" s="41"/>
+    </row>
+    <row r="2" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45" t="s">
+      <c r="I2" s="43"/>
+      <c r="J2" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="42" t="s">
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="N2" s="45" t="s">
+      <c r="N2" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
       <c r="Q2" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="R2" s="45" t="s">
+      <c r="R2" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="S2" s="45"/>
-      <c r="T2" s="45"/>
-      <c r="U2" s="45"/>
-      <c r="V2" s="45" t="s">
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="W2" s="45"/>
-      <c r="X2" s="45"/>
-      <c r="Y2" s="46" t="s">
-        <v>148</v>
-      </c>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="43"/>
-    </row>
-    <row r="3" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="42" t="s">
+      <c r="W2" s="43"/>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z2" s="44" t="s">
+        <v>146</v>
+      </c>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="41"/>
+    </row>
+    <row r="3" spans="1:29" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="40" t="s">
         <v>107</v>
       </c>
       <c r="I3" s="18" t="s">
         <v>18</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="K3" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="K3" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="L3" s="42" t="s">
+      <c r="L3" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="M3" s="42" t="s">
+      <c r="M3" s="40" t="s">
         <v>110</v>
       </c>
       <c r="N3" s="16" t="s">
@@ -1839,22 +1992,25 @@
       <c r="X3" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="Y3" s="15" t="s">
+      <c r="Y3" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z3" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA3" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB3" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="Z3" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="AA3" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="AB3" s="43" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AC3" s="41" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B4" s="17">
         <v>6</v>
@@ -1926,20 +2082,23 @@
         <v>3</v>
       </c>
       <c r="Y4" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="17">
         <v>2</v>
       </c>
-      <c r="Z4" s="17">
-        <v>1</v>
-      </c>
       <c r="AA4" s="17">
         <v>1</v>
       </c>
       <c r="AB4" s="17">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A5" s="49" t="s">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A5" s="47" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="20">
@@ -2011,21 +2170,24 @@
       <c r="X5" s="23">
         <v>0</v>
       </c>
-      <c r="Y5" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="22" t="s">
-        <v>109</v>
+      <c r="Y5" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="24">
+        <v>0</v>
       </c>
       <c r="AA5" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB5" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A6" s="49" t="s">
+      <c r="AB5" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC5" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A6" s="47" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="20">
@@ -2037,11 +2199,11 @@
       <c r="D6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="47" t="s">
+      <c r="E6" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
       <c r="H6" s="19">
         <v>0</v>
       </c>
@@ -2093,21 +2255,24 @@
       <c r="X6" s="23">
         <v>0</v>
       </c>
-      <c r="Y6" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="22" t="s">
-        <v>109</v>
+      <c r="Y6" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="24">
+        <v>0</v>
       </c>
       <c r="AA6" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB6" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A7" s="49" t="s">
+      <c r="AB6" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC6" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A7" s="47" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="20">
@@ -2179,21 +2344,24 @@
       <c r="X7" s="23">
         <v>0</v>
       </c>
-      <c r="Y7" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="22" t="s">
-        <v>109</v>
+      <c r="Y7" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="24">
+        <v>0</v>
       </c>
       <c r="AA7" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB7" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A8" s="49" t="s">
+      <c r="AB7" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC7" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A8" s="47" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="20">
@@ -2205,11 +2373,11 @@
       <c r="D8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="47" t="s">
+      <c r="E8" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
       <c r="H8" s="19">
         <v>0</v>
       </c>
@@ -2261,21 +2429,24 @@
       <c r="X8" s="23">
         <v>0</v>
       </c>
-      <c r="Y8" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="22" t="s">
-        <v>109</v>
+      <c r="Y8" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="24">
+        <v>0</v>
       </c>
       <c r="AA8" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB8" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A9" s="49" t="s">
+      <c r="AB8" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC8" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A9" s="47" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="20">
@@ -2347,21 +2518,24 @@
       <c r="X9" s="23">
         <v>0</v>
       </c>
-      <c r="Y9" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="22" t="s">
-        <v>109</v>
+      <c r="Y9" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="24">
+        <v>0</v>
       </c>
       <c r="AA9" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB9" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A10" s="49" t="s">
+      <c r="AB9" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC9" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A10" s="47" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="20">
@@ -2433,21 +2607,24 @@
       <c r="X10" s="23">
         <v>0</v>
       </c>
-      <c r="Y10" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="22" t="s">
-        <v>109</v>
+      <c r="Y10" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="24">
+        <v>0</v>
       </c>
       <c r="AA10" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB10" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A11" s="49" t="s">
+      <c r="AB10" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC10" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A11" s="47" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="20">
@@ -2519,21 +2696,24 @@
       <c r="X11" s="23">
         <v>0</v>
       </c>
-      <c r="Y11" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="22" t="s">
-        <v>109</v>
+      <c r="Y11" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="24">
+        <v>0</v>
       </c>
       <c r="AA11" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB11" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A12" s="49" t="s">
+      <c r="AB11" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC11" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A12" s="47" t="s">
         <v>35</v>
       </c>
       <c r="B12" s="20">
@@ -2545,11 +2725,11 @@
       <c r="D12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="47" t="s">
+      <c r="E12" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
       <c r="H12" s="19">
         <v>0</v>
       </c>
@@ -2601,21 +2781,24 @@
       <c r="X12" s="23">
         <v>0</v>
       </c>
-      <c r="Y12" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="22" t="s">
-        <v>109</v>
+      <c r="Y12" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="24">
+        <v>0</v>
       </c>
       <c r="AA12" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB12" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A13" s="49" t="s">
+      <c r="AB12" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC12" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A13" s="47" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="20">
@@ -2687,21 +2870,24 @@
       <c r="X13" s="23">
         <v>0</v>
       </c>
-      <c r="Y13" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="22" t="s">
-        <v>109</v>
+      <c r="Y13" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="24">
+        <v>0</v>
       </c>
       <c r="AA13" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB13" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A14" s="49" t="s">
+      <c r="AB13" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC13" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A14" s="47" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="20">
@@ -2713,11 +2899,11 @@
       <c r="D14" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="47" t="s">
+      <c r="E14" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
       <c r="H14" s="19">
         <v>0</v>
       </c>
@@ -2769,21 +2955,24 @@
       <c r="X14" s="23">
         <v>0</v>
       </c>
-      <c r="Y14" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="22" t="s">
-        <v>109</v>
+      <c r="Y14" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="24">
+        <v>0</v>
       </c>
       <c r="AA14" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB14" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A15" s="49" t="s">
+      <c r="AB14" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC14" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A15" s="47" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="20">
@@ -2855,21 +3044,24 @@
       <c r="X15" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y15" s="24">
+      <c r="Y15" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="24">
         <v>11</v>
       </c>
-      <c r="Z15" s="22">
-        <v>0</v>
-      </c>
       <c r="AA15" s="22">
         <v>0</v>
       </c>
-      <c r="AB15" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A16" s="49" t="s">
+      <c r="AB15" s="22">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A16" s="47" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="20">
@@ -2941,21 +3133,24 @@
       <c r="X16" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y16" s="24">
+      <c r="Y16" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="24">
         <v>11</v>
       </c>
-      <c r="Z16" s="22">
-        <v>0</v>
-      </c>
       <c r="AA16" s="22">
         <v>0</v>
       </c>
-      <c r="AB16" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A17" s="49" t="s">
+      <c r="AB16" s="22">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A17" s="47" t="s">
         <v>40</v>
       </c>
       <c r="B17" s="20">
@@ -3027,21 +3222,24 @@
       <c r="X17" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y17" s="24">
+      <c r="Y17" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="24">
         <v>11</v>
       </c>
-      <c r="Z17" s="22">
-        <v>0</v>
-      </c>
       <c r="AA17" s="22">
         <v>0</v>
       </c>
-      <c r="AB17" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A18" s="49" t="s">
+      <c r="AB17" s="22">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A18" s="47" t="s">
         <v>41</v>
       </c>
       <c r="B18" s="20">
@@ -3113,21 +3311,24 @@
       <c r="X18" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y18" s="24">
+      <c r="Y18" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="24">
         <v>11</v>
       </c>
-      <c r="Z18" s="22">
-        <v>0</v>
-      </c>
       <c r="AA18" s="22">
         <v>0</v>
       </c>
-      <c r="AB18" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A19" s="49" t="s">
+      <c r="AB18" s="22">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A19" s="47" t="s">
         <v>42</v>
       </c>
       <c r="B19" s="20">
@@ -3199,21 +3400,24 @@
       <c r="X19" s="23">
         <v>0</v>
       </c>
-      <c r="Y19" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="22" t="s">
-        <v>109</v>
+      <c r="Y19" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="24">
+        <v>0</v>
       </c>
       <c r="AA19" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB19" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A20" s="49" t="s">
+      <c r="AB19" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC19" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A20" s="47" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="20">
@@ -3225,11 +3429,11 @@
       <c r="D20" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="47" t="s">
+      <c r="E20" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
       <c r="H20" s="19">
         <v>0</v>
       </c>
@@ -3281,21 +3485,24 @@
       <c r="X20" s="23">
         <v>0</v>
       </c>
-      <c r="Y20" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="22" t="s">
-        <v>109</v>
+      <c r="Y20" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="24">
+        <v>0</v>
       </c>
       <c r="AA20" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB20" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A21" s="49" t="s">
+      <c r="AB20" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC20" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A21" s="47" t="s">
         <v>44</v>
       </c>
       <c r="B21" s="20">
@@ -3307,11 +3514,11 @@
       <c r="D21" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="47" t="s">
+      <c r="E21" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
       <c r="H21" s="19">
         <v>0</v>
       </c>
@@ -3363,21 +3570,24 @@
       <c r="X21" s="23">
         <v>0</v>
       </c>
-      <c r="Y21" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="22" t="s">
-        <v>109</v>
+      <c r="Y21" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="24">
+        <v>0</v>
       </c>
       <c r="AA21" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB21" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A22" s="49" t="s">
+      <c r="AB21" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC21" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A22" s="47" t="s">
         <v>45</v>
       </c>
       <c r="B22" s="20">
@@ -3449,21 +3659,24 @@
       <c r="X22" s="23">
         <v>0</v>
       </c>
-      <c r="Y22" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="22" t="s">
-        <v>109</v>
+      <c r="Y22" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="24">
+        <v>0</v>
       </c>
       <c r="AA22" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB22" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A23" s="49" t="s">
+      <c r="AB22" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC22" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A23" s="47" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="20">
@@ -3535,21 +3748,24 @@
       <c r="X23" s="23">
         <v>0</v>
       </c>
-      <c r="Y23" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="22" t="s">
-        <v>109</v>
+      <c r="Y23" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="24">
+        <v>0</v>
       </c>
       <c r="AA23" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB23" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A24" s="49" t="s">
+      <c r="AB23" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC23" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A24" s="47" t="s">
         <v>47</v>
       </c>
       <c r="B24" s="20">
@@ -3561,11 +3777,11 @@
       <c r="D24" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="47" t="s">
+      <c r="E24" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
       <c r="H24" s="19">
         <v>0</v>
       </c>
@@ -3617,21 +3833,24 @@
       <c r="X24" s="23">
         <v>0</v>
       </c>
-      <c r="Y24" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z24" s="22" t="s">
-        <v>109</v>
+      <c r="Y24" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="24">
+        <v>0</v>
       </c>
       <c r="AA24" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB24" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A25" s="49" t="s">
+      <c r="AB24" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC24" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A25" s="47" t="s">
         <v>48</v>
       </c>
       <c r="B25" s="20">
@@ -3703,21 +3922,24 @@
       <c r="X25" s="23">
         <v>0</v>
       </c>
-      <c r="Y25" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z25" s="22" t="s">
-        <v>109</v>
+      <c r="Y25" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="24">
+        <v>0</v>
       </c>
       <c r="AA25" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB25" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A26" s="49" t="s">
+      <c r="AB25" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC25" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A26" s="47" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="20">
@@ -3729,11 +3951,11 @@
       <c r="D26" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="47" t="s">
+      <c r="E26" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
       <c r="H26" s="19">
         <v>0</v>
       </c>
@@ -3785,21 +4007,24 @@
       <c r="X26" s="23">
         <v>0</v>
       </c>
-      <c r="Y26" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z26" s="22" t="s">
-        <v>109</v>
+      <c r="Y26" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="24">
+        <v>0</v>
       </c>
       <c r="AA26" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB26" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A27" s="49" t="s">
+      <c r="AB26" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC26" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A27" s="47" t="s">
         <v>50</v>
       </c>
       <c r="B27" s="20">
@@ -3871,21 +4096,24 @@
       <c r="X27" s="23">
         <v>0</v>
       </c>
-      <c r="Y27" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z27" s="22" t="s">
-        <v>109</v>
+      <c r="Y27" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="24">
+        <v>0</v>
       </c>
       <c r="AA27" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB27" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A28" s="49" t="s">
+      <c r="AB27" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC27" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A28" s="47" t="s">
         <v>52</v>
       </c>
       <c r="B28" s="20">
@@ -3957,21 +4185,24 @@
       <c r="X28" s="23">
         <v>0</v>
       </c>
-      <c r="Y28" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z28" s="22" t="s">
-        <v>109</v>
+      <c r="Y28" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="24">
+        <v>0</v>
       </c>
       <c r="AA28" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB28" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A29" s="49" t="s">
+      <c r="AB28" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC28" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A29" s="47" t="s">
         <v>53</v>
       </c>
       <c r="B29" s="20">
@@ -4043,21 +4274,24 @@
       <c r="X29" s="23">
         <v>0</v>
       </c>
-      <c r="Y29" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z29" s="22" t="s">
-        <v>109</v>
+      <c r="Y29" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="24">
+        <v>0</v>
       </c>
       <c r="AA29" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB29" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A30" s="49" t="s">
+      <c r="AB29" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC29" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A30" s="47" t="s">
         <v>54</v>
       </c>
       <c r="B30" s="20">
@@ -4129,21 +4363,24 @@
       <c r="X30" s="23">
         <v>0</v>
       </c>
-      <c r="Y30" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z30" s="22" t="s">
-        <v>109</v>
+      <c r="Y30" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="24">
+        <v>0</v>
       </c>
       <c r="AA30" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB30" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A31" s="49" t="s">
+      <c r="AB30" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC30" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A31" s="47" t="s">
         <v>55</v>
       </c>
       <c r="B31" s="20">
@@ -4215,21 +4452,24 @@
       <c r="X31" s="23">
         <v>0</v>
       </c>
-      <c r="Y31" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z31" s="22" t="s">
-        <v>109</v>
+      <c r="Y31" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="24">
+        <v>0</v>
       </c>
       <c r="AA31" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB31" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A32" s="49" t="s">
+      <c r="AB31" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC31" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A32" s="47" t="s">
         <v>56</v>
       </c>
       <c r="B32" s="20">
@@ -4301,21 +4541,24 @@
       <c r="X32" s="23">
         <v>0</v>
       </c>
-      <c r="Y32" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z32" s="22" t="s">
-        <v>109</v>
+      <c r="Y32" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="24">
+        <v>0</v>
       </c>
       <c r="AA32" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB32" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A33" s="51" t="s">
+      <c r="AB32" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC32" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A33" s="49" t="s">
         <v>5</v>
       </c>
       <c r="B33" s="20">
@@ -4327,11 +4570,11 @@
       <c r="D33" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E33" s="47" t="s">
+      <c r="E33" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
       <c r="H33" s="19">
         <v>1</v>
       </c>
@@ -4383,21 +4626,24 @@
       <c r="X33" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y33" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z33" s="22" t="s">
-        <v>109</v>
+      <c r="Y33" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="24">
+        <v>0</v>
       </c>
       <c r="AA33" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB33" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A34" s="51" t="s">
+      <c r="AB33" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC33" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A34" s="49" t="s">
         <v>6</v>
       </c>
       <c r="B34" s="20">
@@ -4409,11 +4655,11 @@
       <c r="D34" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E34" s="47" t="s">
+      <c r="E34" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
       <c r="H34" s="19">
         <v>1</v>
       </c>
@@ -4465,21 +4711,24 @@
       <c r="X34" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y34" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z34" s="22" t="s">
-        <v>109</v>
+      <c r="Y34" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="24">
+        <v>0</v>
       </c>
       <c r="AA34" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB34" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A35" s="51" t="s">
+      <c r="AB34" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC34" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A35" s="49" t="s">
         <v>9</v>
       </c>
       <c r="B35" s="20">
@@ -4491,11 +4740,11 @@
       <c r="D35" s="12">
         <v>1</v>
       </c>
-      <c r="E35" s="47" t="s">
+      <c r="E35" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
       <c r="H35" s="19">
         <v>1</v>
       </c>
@@ -4547,21 +4796,24 @@
       <c r="X35" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y35" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z35" s="22" t="s">
-        <v>109</v>
+      <c r="Y35" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="24">
+        <v>0</v>
       </c>
       <c r="AA35" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB35" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A36" s="51" t="s">
+      <c r="AB35" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC35" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A36" s="49" t="s">
         <v>10</v>
       </c>
       <c r="B36" s="20">
@@ -4573,11 +4825,11 @@
       <c r="D36" s="12">
         <v>0</v>
       </c>
-      <c r="E36" s="47" t="s">
+      <c r="E36" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
       <c r="H36" s="19">
         <v>1</v>
       </c>
@@ -4629,21 +4881,24 @@
       <c r="X36" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y36" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z36" s="22" t="s">
-        <v>109</v>
+      <c r="Y36" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="24">
+        <v>0</v>
       </c>
       <c r="AA36" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB36" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A37" s="51" t="s">
+      <c r="AB36" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC36" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A37" s="49" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="20">
@@ -4655,11 +4910,11 @@
       <c r="D37" s="12">
         <v>0</v>
       </c>
-      <c r="E37" s="47" t="s">
+      <c r="E37" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F37" s="47"/>
-      <c r="G37" s="47"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
       <c r="H37" s="19">
         <v>1</v>
       </c>
@@ -4711,21 +4966,24 @@
       <c r="X37" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y37" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z37" s="22" t="s">
-        <v>109</v>
+      <c r="Y37" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="24">
+        <v>0</v>
       </c>
       <c r="AA37" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB37" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A38" s="51" t="s">
+      <c r="AB37" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC37" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A38" s="49" t="s">
         <v>14</v>
       </c>
       <c r="B38" s="20">
@@ -4737,11 +4995,11 @@
       <c r="D38" s="12">
         <v>0</v>
       </c>
-      <c r="E38" s="47" t="s">
+      <c r="E38" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
       <c r="H38" s="19">
         <v>1</v>
       </c>
@@ -4793,21 +5051,24 @@
       <c r="X38" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y38" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z38" s="22" t="s">
-        <v>109</v>
+      <c r="Y38" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z38" s="24">
+        <v>0</v>
       </c>
       <c r="AA38" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB38" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A39" s="51" t="s">
+      <c r="AB38" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC38" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A39" s="49" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="20">
@@ -4819,11 +5080,11 @@
       <c r="D39" s="12">
         <v>10001</v>
       </c>
-      <c r="E39" s="47" t="s">
+      <c r="E39" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F39" s="47"/>
-      <c r="G39" s="47"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="45"/>
       <c r="H39" s="19">
         <v>1</v>
       </c>
@@ -4875,21 +5136,24 @@
       <c r="X39" s="23">
         <v>1</v>
       </c>
-      <c r="Y39" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z39" s="22" t="s">
-        <v>109</v>
+      <c r="Y39" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="24">
+        <v>0</v>
       </c>
       <c r="AA39" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB39" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A40" s="51" t="s">
+      <c r="AB39" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC39" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A40" s="49" t="s">
         <v>17</v>
       </c>
       <c r="B40" s="20">
@@ -4901,11 +5165,11 @@
       <c r="D40" s="12">
         <v>10000</v>
       </c>
-      <c r="E40" s="47" t="s">
+      <c r="E40" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="45"/>
       <c r="H40" s="19">
         <v>1</v>
       </c>
@@ -4957,33 +5221,36 @@
       <c r="X40" s="23">
         <v>1</v>
       </c>
-      <c r="Y40" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z40" s="22" t="s">
-        <v>109</v>
+      <c r="Y40" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="24">
+        <v>0</v>
       </c>
       <c r="AA40" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB40" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A41" s="51" t="s">
+      <c r="AB40" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC40" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A41" s="49" t="s">
         <v>57</v>
       </c>
       <c r="B41" s="20">
         <v>10</v>
       </c>
-      <c r="C41" s="47" t="s">
+      <c r="C41" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
       <c r="H41" s="19">
         <v>0</v>
       </c>
@@ -5035,33 +5302,36 @@
       <c r="X41" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y41" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z41" s="22" t="s">
-        <v>109</v>
+      <c r="Y41" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="24">
+        <v>0</v>
       </c>
       <c r="AA41" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB41" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A42" s="51" t="s">
+      <c r="AB41" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC41" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A42" s="49" t="s">
         <v>58</v>
       </c>
       <c r="B42" s="20">
         <v>11</v>
       </c>
-      <c r="C42" s="47" t="s">
+      <c r="C42" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="47"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="45"/>
       <c r="H42" s="19">
         <v>0</v>
       </c>
@@ -5113,21 +5383,24 @@
       <c r="X42" s="23">
         <v>1</v>
       </c>
-      <c r="Y42" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z42" s="22" t="s">
-        <v>109</v>
+      <c r="Y42" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z42" s="24">
+        <v>0</v>
       </c>
       <c r="AA42" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB42" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A43" s="51" t="s">
+      <c r="AB42" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC42" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A43" s="49" t="s">
         <v>59</v>
       </c>
       <c r="B43" s="20">
@@ -5199,21 +5472,24 @@
       <c r="X43" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y43" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z43" s="22" t="s">
-        <v>109</v>
+      <c r="Y43" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="24">
+        <v>0</v>
       </c>
       <c r="AA43" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB43" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A44" s="51" t="s">
+      <c r="AB43" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC43" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A44" s="49" t="s">
         <v>60</v>
       </c>
       <c r="B44" s="20">
@@ -5285,21 +5561,24 @@
       <c r="X44" s="23">
         <v>1</v>
       </c>
-      <c r="Y44" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z44" s="22" t="s">
-        <v>109</v>
+      <c r="Y44" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="24">
+        <v>0</v>
       </c>
       <c r="AA44" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB44" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A45" s="50" t="s">
+      <c r="AB44" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC44" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A45" s="48" t="s">
         <v>61</v>
       </c>
       <c r="B45" s="20">
@@ -5371,21 +5650,24 @@
       <c r="X45" s="23">
         <v>10</v>
       </c>
-      <c r="Y45" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z45" s="22" t="s">
-        <v>109</v>
+      <c r="Y45" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z45" s="24">
+        <v>0</v>
       </c>
       <c r="AA45" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB45" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A46" s="50" t="s">
+      <c r="AB45" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC45" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A46" s="48" t="s">
         <v>62</v>
       </c>
       <c r="B46" s="20">
@@ -5457,20 +5739,23 @@
       <c r="X46" s="23">
         <v>11</v>
       </c>
-      <c r="Y46" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z46" s="22" t="s">
-        <v>109</v>
+      <c r="Y46" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="24">
+        <v>0</v>
       </c>
       <c r="AA46" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB46" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB46" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC46" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A47" s="32" t="s">
         <v>63</v>
       </c>
@@ -5543,20 +5828,23 @@
       <c r="X47" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y47" s="24">
+      <c r="Y47" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="24">
         <v>10</v>
       </c>
-      <c r="Z47" s="22">
-        <v>1</v>
-      </c>
-      <c r="AA47" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="AB47" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA47" s="22">
+        <v>1</v>
+      </c>
+      <c r="AB47" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC47" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A48" s="32" t="s">
         <v>64</v>
       </c>
@@ -5629,32 +5917,35 @@
       <c r="X48" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y48" s="24">
-        <v>1</v>
-      </c>
-      <c r="Z48" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA48" s="22">
-        <v>1</v>
-      </c>
-      <c r="AB48" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="Y48" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="24">
+        <v>1</v>
+      </c>
+      <c r="AA48" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB48" s="22">
+        <v>1</v>
+      </c>
+      <c r="AC48" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A49" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B49" s="20">
         <v>0</v>
       </c>
-      <c r="C49" s="47" t="s">
+      <c r="C49" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="D49" s="47"/>
-      <c r="E49" s="47"/>
-      <c r="F49" s="47"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="45"/>
       <c r="G49" s="20">
         <v>1101</v>
       </c>
@@ -5709,32 +6000,35 @@
       <c r="X49" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y49" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z49" s="22" t="s">
-        <v>109</v>
+      <c r="Y49" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z49" s="24">
+        <v>0</v>
       </c>
       <c r="AA49" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB49" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB49" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC49" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="s">
         <v>67</v>
       </c>
       <c r="B50" s="20">
         <v>0</v>
       </c>
-      <c r="C50" s="47" t="s">
+      <c r="C50" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="D50" s="47"/>
-      <c r="E50" s="47"/>
-      <c r="F50" s="47"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
       <c r="G50" s="20">
         <v>1100</v>
       </c>
@@ -5789,20 +6083,23 @@
       <c r="X50" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y50" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z50" s="22" t="s">
-        <v>109</v>
+      <c r="Y50" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z50" s="24">
+        <v>0</v>
       </c>
       <c r="AA50" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB50" s="24">
+      <c r="AB50" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC50" s="24">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
         <v>68</v>
       </c>
@@ -5815,11 +6112,11 @@
       <c r="D51" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E51" s="47" t="s">
+      <c r="E51" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F51" s="47"/>
-      <c r="G51" s="47"/>
+      <c r="F51" s="45"/>
+      <c r="G51" s="45"/>
       <c r="H51" s="19">
         <v>0</v>
       </c>
@@ -5871,20 +6168,23 @@
       <c r="X51" s="23">
         <v>100</v>
       </c>
-      <c r="Y51" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z51" s="22" t="s">
-        <v>109</v>
+      <c r="Y51" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z51" s="24">
+        <v>0</v>
       </c>
       <c r="AA51" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB51" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB51" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC51" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
         <v>69</v>
       </c>
@@ -5897,11 +6197,11 @@
       <c r="D52" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E52" s="47" t="s">
+      <c r="E52" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F52" s="47"/>
-      <c r="G52" s="47"/>
+      <c r="F52" s="45"/>
+      <c r="G52" s="45"/>
       <c r="H52" s="19">
         <v>0</v>
       </c>
@@ -5953,20 +6253,23 @@
       <c r="X52" s="23">
         <v>100</v>
       </c>
-      <c r="Y52" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z52" s="22" t="s">
-        <v>109</v>
+      <c r="Y52" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z52" s="24">
+        <v>0</v>
       </c>
       <c r="AA52" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB52" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB52" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC52" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A53" s="19" t="s">
         <v>70</v>
       </c>
@@ -5979,11 +6282,11 @@
       <c r="D53" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E53" s="47" t="s">
+      <c r="E53" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F53" s="47"/>
-      <c r="G53" s="47"/>
+      <c r="F53" s="45"/>
+      <c r="G53" s="45"/>
       <c r="H53" s="19">
         <v>0</v>
       </c>
@@ -6035,20 +6338,23 @@
       <c r="X53" s="23">
         <v>100</v>
       </c>
-      <c r="Y53" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z53" s="22" t="s">
-        <v>109</v>
+      <c r="Y53" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z53" s="24">
+        <v>0</v>
       </c>
       <c r="AA53" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB53" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB53" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC53" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="s">
         <v>71</v>
       </c>
@@ -6061,11 +6367,11 @@
       <c r="D54" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E54" s="47" t="s">
+      <c r="E54" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F54" s="47"/>
-      <c r="G54" s="47"/>
+      <c r="F54" s="45"/>
+      <c r="G54" s="45"/>
       <c r="H54" s="19">
         <v>0</v>
       </c>
@@ -6117,20 +6423,23 @@
       <c r="X54" s="23">
         <v>100</v>
       </c>
-      <c r="Y54" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z54" s="22" t="s">
-        <v>109</v>
+      <c r="Y54" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z54" s="24">
+        <v>0</v>
       </c>
       <c r="AA54" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB54" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB54" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC54" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="s">
         <v>72</v>
       </c>
@@ -6143,11 +6452,11 @@
       <c r="D55" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E55" s="47" t="s">
+      <c r="E55" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F55" s="47"/>
-      <c r="G55" s="47"/>
+      <c r="F55" s="45"/>
+      <c r="G55" s="45"/>
       <c r="H55" s="19">
         <v>0</v>
       </c>
@@ -6199,20 +6508,23 @@
       <c r="X55" s="23">
         <v>100</v>
       </c>
-      <c r="Y55" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z55" s="22" t="s">
-        <v>109</v>
+      <c r="Y55" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z55" s="24">
+        <v>0</v>
       </c>
       <c r="AA55" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB55" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB55" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC55" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
         <v>73</v>
       </c>
@@ -6225,11 +6537,11 @@
       <c r="D56" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E56" s="47" t="s">
+      <c r="E56" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F56" s="47"/>
-      <c r="G56" s="47"/>
+      <c r="F56" s="45"/>
+      <c r="G56" s="45"/>
       <c r="H56" s="19">
         <v>0</v>
       </c>
@@ -6281,20 +6593,23 @@
       <c r="X56" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y56" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z56" s="22" t="s">
-        <v>109</v>
+      <c r="Y56" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z56" s="24">
+        <v>0</v>
       </c>
       <c r="AA56" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB56" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB56" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC56" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="s">
         <v>74</v>
       </c>
@@ -6307,11 +6622,11 @@
       <c r="D57" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E57" s="47" t="s">
+      <c r="E57" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F57" s="47"/>
-      <c r="G57" s="47"/>
+      <c r="F57" s="45"/>
+      <c r="G57" s="45"/>
       <c r="H57" s="19">
         <v>0</v>
       </c>
@@ -6363,20 +6678,23 @@
       <c r="X57" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y57" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z57" s="22" t="s">
-        <v>109</v>
+      <c r="Y57" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z57" s="24">
+        <v>0</v>
       </c>
       <c r="AA57" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB57" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB57" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC57" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
         <v>75</v>
       </c>
@@ -6389,11 +6707,11 @@
       <c r="D58" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E58" s="47" t="s">
+      <c r="E58" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F58" s="47"/>
-      <c r="G58" s="47"/>
+      <c r="F58" s="45"/>
+      <c r="G58" s="45"/>
       <c r="H58" s="19">
         <v>0</v>
       </c>
@@ -6445,20 +6763,23 @@
       <c r="X58" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y58" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z58" s="22" t="s">
-        <v>109</v>
+      <c r="Y58" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z58" s="24">
+        <v>0</v>
       </c>
       <c r="AA58" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB58" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB58" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC58" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A59" s="19" t="s">
         <v>76</v>
       </c>
@@ -6531,21 +6852,24 @@
       <c r="X59" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y59" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z59" s="22" t="s">
-        <v>109</v>
+      <c r="Y59" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z59" s="24">
+        <v>0</v>
       </c>
       <c r="AA59" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB59" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A60" s="50" t="s">
+      <c r="AB59" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC59" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A60" s="48" t="s">
         <v>78</v>
       </c>
       <c r="B60" s="20">
@@ -6617,20 +6941,23 @@
       <c r="X60" s="23">
         <v>101</v>
       </c>
-      <c r="Y60" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z60" s="22" t="s">
-        <v>109</v>
+      <c r="Y60" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z60" s="24">
+        <v>0</v>
       </c>
       <c r="AA60" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB60" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB60" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC60" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A61" s="32" t="s">
         <v>79</v>
       </c>
@@ -6703,22 +7030,25 @@
       <c r="X61" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y61" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z61" s="22" t="s">
-        <v>109</v>
+      <c r="Y61" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z61" s="24">
+        <v>0</v>
       </c>
       <c r="AA61" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB61" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB61" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC61" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A62" s="19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H62" s="19">
         <v>0</v>
@@ -6771,16 +7101,19 @@
       <c r="X62" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="Y62" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z62" s="22" t="s">
-        <v>109</v>
+      <c r="Y62" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z62" s="24">
+        <v>0</v>
       </c>
       <c r="AA62" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="AB62" s="24">
+      <c r="AB62" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC62" s="24">
         <v>11</v>
       </c>
     </row>
@@ -6820,62 +7153,14 @@
     <mergeCell ref="N2:P2"/>
     <mergeCell ref="R2:U2"/>
     <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="V1:AA1"/>
+    <mergeCell ref="V1:AB1"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="R1:U1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="V1:V61 V63:V1048576">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N61 N63:N1048576">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V62">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N62">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -6893,12 +7178,12 @@
     <col min="2" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="B1" s="44" t="s">
-        <v>178</v>
+        <v>174</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -6906,7 +7191,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -6930,7 +7215,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -6943,8 +7228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D6B0BF-8614-43A7-9F15-E4FE95337B3D}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6960,10 +7245,10 @@
       <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="48"/>
+      <c r="B1" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="46"/>
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
@@ -7054,7 +7339,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7077,11 +7362,11 @@
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="B1" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
@@ -7144,7 +7429,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J3" s="1">
         <v>1</v>
@@ -7447,10 +7732,78 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780E22FF-6159-4733-93EB-5184B9746FE9}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.125" style="1"/>
+    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="27">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="27">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="27">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" s="27">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{947260C0-B57D-402D-A7FB-E56302B48C32}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7522,7 +7875,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>138</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -7530,7 +7883,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>139</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -7538,7 +7891,7 @@
         <v>100</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -7546,73 +7899,7 @@
         <v>101</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780E22FF-6159-4733-93EB-5184B9746FE9}">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.125" style="1"/>
-    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="27">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D2" s="27">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="27">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D3" s="27">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>